<commit_message>
calc from line zero
</commit_message>
<xml_diff>
--- a/tests/indicators/s-z/T3/T3.Calc.xlsx
+++ b/tests/indicators/s-z/T3/T3.Calc.xlsx
@@ -4,9 +4,9 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A105CE45-1E71-4A50-8660-9581D0928CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E512AD00-5C5E-4FE1-AC10-142C58D24B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23100" yWindow="2400" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T3" sheetId="1" r:id="rId1"/>
@@ -1515,7 +1515,9 @@
       <c r="N2" s="2">
         <v>42738</v>
       </c>
-      <c r="O2" s="7"/>
+      <c r="O2" s="7">
+        <v>212.8</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
@@ -1561,7 +1563,9 @@
       <c r="N3" s="2">
         <v>42739</v>
       </c>
-      <c r="O3" s="7"/>
+      <c r="O3" s="7">
+        <v>212.94720000000001</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -1604,7 +1608,9 @@
       <c r="N4" s="2">
         <v>42740</v>
       </c>
-      <c r="O4" s="7"/>
+      <c r="O4" s="7">
+        <v>213.17500000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -1650,7 +1656,9 @@
       <c r="N5" s="2">
         <v>42741</v>
       </c>
-      <c r="O5" s="7"/>
+      <c r="O5" s="7">
+        <v>213.5042</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -1696,7 +1704,9 @@
       <c r="N6" s="2">
         <v>42744</v>
       </c>
-      <c r="O6" s="7"/>
+      <c r="O6" s="7">
+        <v>213.78020000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
@@ -1746,7 +1756,9 @@
       <c r="N7" s="2">
         <v>42745</v>
       </c>
-      <c r="O7" s="7"/>
+      <c r="O7" s="8">
+        <v>213.96539999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -1796,7 +1808,9 @@
       <c r="N8" s="2">
         <v>42746</v>
       </c>
-      <c r="O8" s="7"/>
+      <c r="O8" s="7">
+        <v>214.1386</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -1846,7 +1860,9 @@
       <c r="N9" s="2">
         <v>42747</v>
       </c>
-      <c r="O9" s="7"/>
+      <c r="O9" s="7">
+        <v>214.2379</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -1896,7 +1912,9 @@
       <c r="N10" s="2">
         <v>42748</v>
       </c>
-      <c r="O10" s="7"/>
+      <c r="O10" s="7">
+        <v>214.3263</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -1939,7 +1957,9 @@
       <c r="N11" s="2">
         <v>42752</v>
       </c>
-      <c r="O11" s="7"/>
+      <c r="O11" s="7">
+        <v>214.3202</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -1982,7 +2002,9 @@
       <c r="N12" s="2">
         <v>42753</v>
       </c>
-      <c r="O12" s="7"/>
+      <c r="O12" s="7">
+        <v>214.29560000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -2025,7 +2047,9 @@
       <c r="N13" s="2">
         <v>42754</v>
       </c>
-      <c r="O13" s="7"/>
+      <c r="O13" s="7">
+        <v>214.18299999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
@@ -2068,7 +2092,9 @@
       <c r="N14" s="2">
         <v>42755</v>
       </c>
-      <c r="O14" s="7"/>
+      <c r="O14" s="7">
+        <v>214.1063</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
@@ -2111,7 +2137,9 @@
       <c r="N15" s="2">
         <v>42758</v>
       </c>
-      <c r="O15" s="7"/>
+      <c r="O15" s="7">
+        <v>214.01730000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -2154,7 +2182,9 @@
       <c r="N16" s="2">
         <v>42759</v>
       </c>
-      <c r="O16" s="7"/>
+      <c r="O16" s="7">
+        <v>214.0805</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -2197,7 +2227,9 @@
       <c r="N17" s="2">
         <v>42760</v>
       </c>
-      <c r="O17" s="7"/>
+      <c r="O17" s="7">
+        <v>214.47630000000001</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -2240,7 +2272,9 @@
       <c r="N18" s="2">
         <v>42761</v>
       </c>
-      <c r="O18" s="7"/>
+      <c r="O18" s="7">
+        <v>215.03630000000001</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
@@ -2283,7 +2317,9 @@
       <c r="N19" s="2">
         <v>42762</v>
       </c>
-      <c r="O19" s="7"/>
+      <c r="O19" s="7">
+        <v>215.56379999999999</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -2326,7 +2362,9 @@
       <c r="N20" s="2">
         <v>42765</v>
       </c>
-      <c r="O20" s="7"/>
+      <c r="O20" s="7">
+        <v>215.82169999999999</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -2369,7 +2407,9 @@
       <c r="N21" s="2">
         <v>42766</v>
       </c>
-      <c r="O21" s="7"/>
+      <c r="O21" s="7">
+        <v>215.8424</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
@@ -2412,7 +2452,9 @@
       <c r="N22" s="2">
         <v>42767</v>
       </c>
-      <c r="O22" s="7"/>
+      <c r="O22" s="7">
+        <v>215.73320000000001</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -2455,7 +2497,9 @@
       <c r="N23" s="2">
         <v>42768</v>
       </c>
-      <c r="O23" s="7"/>
+      <c r="O23" s="7">
+        <v>215.5917</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -2498,7 +2542,9 @@
       <c r="N24" s="2">
         <v>42769</v>
       </c>
-      <c r="O24" s="7"/>
+      <c r="O24" s="7">
+        <v>215.63489999999999</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -2541,7 +2587,9 @@
       <c r="N25" s="2">
         <v>42772</v>
       </c>
-      <c r="O25" s="8"/>
+      <c r="O25" s="7">
+        <v>215.7774</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -2585,7 +2633,7 @@
         <v>42773</v>
       </c>
       <c r="O26" s="8">
-        <v>215.93430000000001</v>
+        <v>215.94810000000001</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -2630,7 +2678,7 @@
         <v>42774</v>
       </c>
       <c r="O27" s="7">
-        <v>216.1284</v>
+        <v>216.1371</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -2675,7 +2723,7 @@
         <v>42775</v>
       </c>
       <c r="O28" s="7">
-        <v>216.45830000000001</v>
+        <v>216.46379999999999</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -2720,7 +2768,7 @@
         <v>42776</v>
       </c>
       <c r="O29" s="7">
-        <v>216.95689999999999</v>
+        <v>216.96029999999999</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -2765,7 +2813,7 @@
         <v>42779</v>
       </c>
       <c r="O30" s="7">
-        <v>217.64769999999999</v>
+        <v>217.6497</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -2810,7 +2858,7 @@
         <v>42780</v>
       </c>
       <c r="O31" s="7">
-        <v>218.4862</v>
+        <v>218.48750000000001</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -2855,7 +2903,7 @@
         <v>42781</v>
       </c>
       <c r="O32" s="7">
-        <v>219.44839999999999</v>
+        <v>219.44909999999999</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2900,7 +2948,7 @@
         <v>42782</v>
       </c>
       <c r="O33" s="7">
-        <v>220.35300000000001</v>
+        <v>220.35339999999999</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -2945,7 +2993,7 @@
         <v>42783</v>
       </c>
       <c r="O34" s="7">
-        <v>221.1301</v>
+        <v>221.13030000000001</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -2990,7 +3038,7 @@
         <v>42787</v>
       </c>
       <c r="O35" s="7">
-        <v>221.88579999999999</v>
+        <v>221.88589999999999</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>